<commit_message>
Fixing the import bugs and adding tests
</commit_message>
<xml_diff>
--- a/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/teacher_good_sheet.xlsx
+++ b/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/teacher_good_sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manchuck/PhpstormProjects/Cmwn/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitu/Documents/cmwn-platform/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="1120" windowWidth="21560" windowHeight="16840" activeTab="2"/>
+    <workbookView xWindow="3800" yWindow="460" windowWidth="21560" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Teachers" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>01X100</t>
   </si>
   <si>
-    <t>Assistant Principal</t>
-  </si>
-  <si>
     <t>Carol</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
       </rPr>
       <t>kind@gmail.com</t>
     </r>
+  </si>
+  <si>
+    <t>Asst Principal</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="194" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1195,17 +1195,17 @@
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>6</v>
@@ -1465,20 +1465,20 @@
         <v>14</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>13</v>
@@ -1737,17 +1737,17 @@
         <v>14</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>6</v>
@@ -2009,17 +2009,17 @@
         <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>6</v>
@@ -2281,17 +2281,17 @@
         <v>14</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>6</v>
@@ -2553,20 +2553,20 @@
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="G8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>13</v>
@@ -2825,20 +2825,20 @@
         <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="G9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="13"/>
@@ -3095,20 +3095,20 @@
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="G10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="13"/>
@@ -3365,17 +3365,17 @@
         <v>14</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>6</v>
@@ -3664,7 +3664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>